<commit_message>
added better colour theme
</commit_message>
<xml_diff>
--- a/sample_v0.2.xlsx
+++ b/sample_v0.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonnyl\Downloads\DiffXcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3695D3F0-2961-4EB2-8145-85D144ECFB58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA3FCD4-44F0-4607-B341-E4B262ED7BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1278,8 +1278,8 @@
   <dimension ref="A1:E391"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1420,7 +1420,7 @@
         <v>456</v>
       </c>
       <c r="C8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D8">
         <v>2011</v>
@@ -1471,7 +1471,7 @@
         <v>789</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D11">
         <v>2011</v>
@@ -1502,7 +1502,7 @@
         <v>31</v>
       </c>
       <c r="B13">
-        <v>456</v>
+        <v>789</v>
       </c>
       <c r="C13" t="s">
         <v>135</v>
@@ -1525,7 +1525,7 @@
         <v>135</v>
       </c>
       <c r="D14">
-        <v>2011</v>
+        <v>2013</v>
       </c>
       <c r="E14" s="1">
         <v>48112.764779075267</v>
@@ -1621,7 +1621,7 @@
         <v>0</v>
       </c>
       <c r="B20">
-        <v>456</v>
+        <v>123</v>
       </c>
       <c r="C20" t="s">
         <v>135</v>

</xml_diff>